<commit_message>
Final major code push
lots of stuff - final analyses and figures.
</commit_message>
<xml_diff>
--- a/output/SupplementaryTable2-pretty.xlsx
+++ b/output/SupplementaryTable2-pretty.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicablois/Documents/GitHub/LaBrea_smallmamm_isotopes/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{F6CC322D-59AC-A44D-8060-2FC0AD4743B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1DA682-CAF2-AA47-AE91-B922005B300B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SupplementaryTable2" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -883,17 +883,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>